<commit_message>
extract chart function implemented and tested half way
</commit_message>
<xml_diff>
--- a/imev0/test2.xlsx
+++ b/imev0/test2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="140" windowWidth="16540" windowHeight="13940"/>
+    <workbookView xWindow="120" yWindow="140" windowWidth="22400" windowHeight="13040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4161" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4160" uniqueCount="294">
   <si>
     <t>تاریخ</t>
   </si>
@@ -1772,13 +1772,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z322"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="A1:Z322"/>
+    <sheetView tabSelected="1" topLeftCell="A310" workbookViewId="0">
+      <selection activeCell="A1909" sqref="A323:XFD1909"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
@@ -23033,9 +23033,7 @@
       </c>
     </row>
     <row r="285" spans="1:26" ht="16">
-      <c r="A285" s="4" t="s">
-        <v>46</v>
-      </c>
+      <c r="A285" s="4"/>
       <c r="B285" s="4" t="s">
         <v>54</v>
       </c>

</xml_diff>